<commit_message>
Add studies to readme
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Box\ColoradoRiver\LakeMeadInflow\Myers-Rosenberg\ReservoirInflowBlogPost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E25BD0C-5E00-464A-A59B-4DE68A68EB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F5CC17-9CBD-44E4-9A69-B7B8468A2723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,36 +502,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Starting to edit R file
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F5CC17-9CBD-44E4-9A69-B7B8468A2723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896F27D7-C2DF-43D3-83AF-0899F93D8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Flow Type</t>
   </si>
@@ -72,45 +72,18 @@
     <t>https://californiawaterblog.com/2023/01/08/drought-and-the-colorado-river-localizing-water-in-los-angeles/</t>
   </si>
   <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Capped depletions to inflows over a lookback period of 10 years</t>
-  </si>
-  <si>
-    <t>Immersive modeling for Lake Powell-Lake Mead water bank (2021)</t>
-  </si>
-  <si>
-    <t>Adapted consumption to reservior inflow and evaporation</t>
-  </si>
-  <si>
     <t>Lee Ferry</t>
   </si>
   <si>
     <t>Flow Location</t>
   </si>
   <si>
-    <t>Release 95% of inflow</t>
-  </si>
-  <si>
-    <t>Powell</t>
-  </si>
-  <si>
-    <t>Mead</t>
-  </si>
-  <si>
     <t>Glen Canyon Dam</t>
   </si>
   <si>
     <t>Release</t>
   </si>
   <si>
-    <t>Release to stabilize Lake Powell level</t>
-  </si>
-  <si>
-    <t>Reanalysis of Reclamation's ensembles and traces</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Lowest consecutive 10-year flow</t>
   </si>
   <si>
@@ -118,6 +91,54 @@
   </si>
   <si>
     <t xml:space="preserve">   Lowest consecutive 3-year flow.</t>
+  </si>
+  <si>
+    <t>Extreme Low Flow Method</t>
+  </si>
+  <si>
+    <t>A. From tree rings back to 1400 AD</t>
+  </si>
+  <si>
+    <t>B. Collaborator choices in immersive modeling sessions</t>
+  </si>
+  <si>
+    <t>C.Low Lake Powell releases + gains through Grand Canyon</t>
+  </si>
+  <si>
+    <t>D. 85%, 65%, and 50% of 2000 to 2018 flow</t>
+  </si>
+  <si>
+    <t>F. Extreme low flows from Reclamation's ensembles and traces</t>
+  </si>
+  <si>
+    <t>Strategy to Stabilize Lake Levels</t>
+  </si>
+  <si>
+    <t>Release to prevent drawdown to 3,490 feet.</t>
+  </si>
+  <si>
+    <t>Release 95% of regulated inflow.</t>
+  </si>
+  <si>
+    <t>Divide inflow; Users consume and conserve within their account balance.</t>
+  </si>
+  <si>
+    <t>Cap depletions to 10-year lookback period of flow.</t>
+  </si>
+  <si>
+    <t>Rule curve; Consumption equals or less than inflow minus evaporation.</t>
+  </si>
+  <si>
+    <t>Immersive modeling in progress</t>
+  </si>
+  <si>
+    <t>E. Reclamation's Post 2026 web tool</t>
+  </si>
+  <si>
+    <t>Lake Mead</t>
+  </si>
+  <si>
+    <t>Lake Powell</t>
   </si>
 </sst>
 </file>
@@ -468,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,182 +502,214 @@
     <col min="3" max="3" width="11.6328125" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5">
         <v>6</v>
       </c>
-      <c r="E6" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="5">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E9" s="5">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>7.1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5">
-        <v>4.0999999999999996</v>
+        <v>3.9</v>
       </c>
       <c r="E10" s="5">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5">
-        <v>3.9</v>
-      </c>
-      <c r="E11" s="5">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="18" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Read in Excel file sheet
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896F27D7-C2DF-43D3-83AF-0899F93D8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9225E3BE-0103-4E71-8680-60921EBBDCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
     <sheet name="BasinWaterAccounts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Flow Type</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Session</t>
   </si>
   <si>
-    <t>Erik - Colorado River Blog post</t>
-  </si>
-  <si>
-    <t>https://californiawaterblog.com/2023/01/08/drought-and-the-colorado-river-localizing-water-in-los-angeles/</t>
-  </si>
-  <si>
     <t>Lee Ferry</t>
   </si>
   <si>
@@ -84,15 +78,6 @@
     <t>Release</t>
   </si>
   <si>
-    <t xml:space="preserve">   Lowest consecutive 10-year flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Lowest consecutive 4-year flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Lowest consecutive 3-year flow.</t>
-  </si>
-  <si>
     <t>Extreme Low Flow Method</t>
   </si>
   <si>
@@ -139,6 +124,18 @@
   </si>
   <si>
     <t>Lake Powell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Lowest consecutive 10-year flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Lowest consecutive 4-year flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Lowest consecutive 3-year flow.</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -188,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,10 +507,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -522,15 +522,15 @@
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -542,15 +542,15 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -562,15 +562,15 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
@@ -582,15 +582,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>3</v>
@@ -602,18 +602,18 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5">
         <v>4</v>
@@ -622,28 +622,35 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -655,15 +662,15 @@
         <v>7.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -675,15 +682,15 @@
         <v>7.1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -695,22 +702,7 @@
         <v>6.8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="17" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of segment plot
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9225E3BE-0103-4E71-8680-60921EBBDCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1995EA84-23FB-418F-B85F-3AA9014F8E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Minimum (maf)</t>
   </si>
   <si>
-    <t>Maximim (maf)</t>
-  </si>
-  <si>
     <t>Regulated</t>
   </si>
   <si>
@@ -90,12 +87,6 @@
     <t>C.Low Lake Powell releases + gains through Grand Canyon</t>
   </si>
   <si>
-    <t>D. 85%, 65%, and 50% of 2000 to 2018 flow</t>
-  </si>
-  <si>
-    <t>F. Extreme low flows from Reclamation's ensembles and traces</t>
-  </si>
-  <si>
     <t>Strategy to Stabilize Lake Levels</t>
   </si>
   <si>
@@ -126,16 +117,25 @@
     <t>Lake Powell</t>
   </si>
   <si>
-    <t xml:space="preserve">       Lowest consecutive 10-year flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Lowest consecutive 4-year flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       Lowest consecutive 3-year flow.</t>
-  </si>
-  <si>
     <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">       10-year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       4-year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       3-year</t>
+  </si>
+  <si>
+    <t>D. 85%, 65%, and 50% of 2000 to 2018 average flow</t>
+  </si>
+  <si>
+    <t>F. Lowest consecutive flows in Reclamation's ensembles and traces</t>
+  </si>
+  <si>
+    <t>Maximum (maf)</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,16 +501,16 @@
     <col min="2" max="2" width="12.7265625" customWidth="1"/>
     <col min="3" max="3" width="11.6328125" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="9.81640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -519,21 +519,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="5">
         <v>5</v>
@@ -542,18 +542,18 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -562,18 +562,18 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5">
         <v>7</v>
@@ -582,18 +582,18 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5">
         <v>6</v>
@@ -602,18 +602,18 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D6" s="5">
         <v>4</v>
@@ -622,18 +622,18 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -642,18 +642,18 @@
         <v>0</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="5">
         <v>5</v>
@@ -662,18 +662,18 @@
         <v>7.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="5">
         <v>4.0999999999999996</v>
@@ -682,18 +682,18 @@
         <v>7.1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5">
         <v>3.9</v>
@@ -702,7 +702,7 @@
         <v>6.8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -722,18 +722,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
x-axis label printing correctly
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1995EA84-23FB-418F-B85F-3AA9014F8E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24D5B28-A484-436D-ABAF-F1B0DF9919BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,61 +81,61 @@
     <t>A. From tree rings back to 1400 AD</t>
   </si>
   <si>
+    <t>Strategy to Stabilize Lake Levels</t>
+  </si>
+  <si>
+    <t>Release to prevent drawdown to 3,490 feet.</t>
+  </si>
+  <si>
+    <t>Release 95% of regulated inflow.</t>
+  </si>
+  <si>
+    <t>Divide inflow; Users consume and conserve within their account balance.</t>
+  </si>
+  <si>
+    <t>Cap depletions to 10-year lookback period of flow.</t>
+  </si>
+  <si>
+    <t>Rule curve; Consumption equals or less than inflow minus evaporation.</t>
+  </si>
+  <si>
+    <t>Immersive modeling in progress</t>
+  </si>
+  <si>
+    <t>E. Reclamation's Post 2026 web tool</t>
+  </si>
+  <si>
+    <t>Lake Mead</t>
+  </si>
+  <si>
+    <t>Lake Powell</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Maximum (maf)</t>
+  </si>
+  <si>
+    <t>F1. 10-year</t>
+  </si>
+  <si>
+    <t>F2. 4-year</t>
+  </si>
+  <si>
+    <t>F3. 3-year</t>
+  </si>
+  <si>
     <t>B. Collaborator choices in immersive modeling sessions</t>
   </si>
   <si>
-    <t>C.Low Lake Powell releases + gains through Grand Canyon</t>
-  </si>
-  <si>
-    <t>Strategy to Stabilize Lake Levels</t>
-  </si>
-  <si>
-    <t>Release to prevent drawdown to 3,490 feet.</t>
-  </si>
-  <si>
-    <t>Release 95% of regulated inflow.</t>
-  </si>
-  <si>
-    <t>Divide inflow; Users consume and conserve within their account balance.</t>
-  </si>
-  <si>
-    <t>Cap depletions to 10-year lookback period of flow.</t>
-  </si>
-  <si>
-    <t>Rule curve; Consumption equals or less than inflow minus evaporation.</t>
-  </si>
-  <si>
-    <t>Immersive modeling in progress</t>
-  </si>
-  <si>
-    <t>E. Reclamation's Post 2026 web tool</t>
-  </si>
-  <si>
-    <t>Lake Mead</t>
-  </si>
-  <si>
-    <t>Lake Powell</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">       10-year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       4-year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       3-year</t>
+    <t>C. Low Lake Powell releases + gains through Grand Canyon</t>
   </si>
   <si>
     <t>D. 85%, 65%, and 50% of 2000 to 2018 average flow</t>
   </si>
   <si>
     <t>F. Lowest consecutive flows in Reclamation's ensembles and traces</t>
-  </si>
-  <si>
-    <t>Maximum (maf)</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -542,12 +542,12 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -562,15 +562,15 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -582,15 +582,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -602,12 +602,12 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -622,12 +622,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -642,12 +642,12 @@
         <v>0</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -662,12 +662,12 @@
         <v>7.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -682,12 +682,12 @@
         <v>7.1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -702,7 +702,7 @@
         <v>6.8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have second right axis of strategy working
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24D5B28-A484-436D-ABAF-F1B0DF9919BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79346A57-8C93-4E73-AE05-73FD034833ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Flow Type</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Lake Powell</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Maximum (maf)</t>
@@ -492,7 +489,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>14</v>
@@ -547,7 +544,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -567,7 +564,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>22</v>
@@ -587,7 +584,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -627,7 +624,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -641,13 +638,11 @@
       <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -667,7 +662,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -687,7 +682,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Working to split strings on inflow methods; output USGS Lake Mead inflow calc to CSV
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79346A57-8C93-4E73-AE05-73FD034833ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1152F784-4D48-46DB-B73E-F46578F1570F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
@@ -84,27 +84,9 @@
     <t>Strategy to Stabilize Lake Levels</t>
   </si>
   <si>
-    <t>Release to prevent drawdown to 3,490 feet.</t>
-  </si>
-  <si>
-    <t>Release 95% of regulated inflow.</t>
-  </si>
-  <si>
-    <t>Divide inflow; Users consume and conserve within their account balance.</t>
-  </si>
-  <si>
-    <t>Cap depletions to 10-year lookback period of flow.</t>
-  </si>
-  <si>
-    <t>Rule curve; Consumption equals or less than inflow minus evaporation.</t>
-  </si>
-  <si>
     <t>Immersive modeling in progress</t>
   </si>
   <si>
-    <t>E. Reclamation's Post 2026 web tool</t>
-  </si>
-  <si>
     <t>Lake Mead</t>
   </si>
   <si>
@@ -123,16 +105,34 @@
     <t>F3. 3-year</t>
   </si>
   <si>
-    <t>B. Collaborator choices in immersive modeling sessions</t>
-  </si>
-  <si>
-    <t>C. Low Lake Powell releases + gains through Grand Canyon</t>
-  </si>
-  <si>
-    <t>D. 85%, 65%, and 50% of 2000 to 2018 average flow</t>
-  </si>
-  <si>
-    <t>F. Lowest consecutive flows in Reclamation's ensembles and traces</t>
+    <t>B. Collaborator choices in immersive  modeling sessions</t>
+  </si>
+  <si>
+    <t>C. Low Lake Powell releases + gains  through Grand Canyon</t>
+  </si>
+  <si>
+    <t>D. 85%, 65%, and 50% of 2000 to 2018  average flow</t>
+  </si>
+  <si>
+    <t>E. Reclamation's Post 2026  web tool</t>
+  </si>
+  <si>
+    <t>F. Lowest consecutive flows in Reclamation's  ensembles and traces</t>
+  </si>
+  <si>
+    <t>Cap depletions to 10-year lookback  period of flow.</t>
+  </si>
+  <si>
+    <t>Divide inflow; Users consume and conserve  within their account balance.</t>
+  </si>
+  <si>
+    <t>Rule curve; Consumption equals or less  than inflow minus evaporation.</t>
+  </si>
+  <si>
+    <t>Release 95% of regulated  inflow.</t>
+  </si>
+  <si>
+    <t>Release to prevent drawdown  to 3,490 feet.</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>14</v>
@@ -539,12 +539,12 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -559,15 +559,15 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -579,15 +579,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -599,12 +599,12 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -619,12 +619,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -657,12 +657,12 @@
         <v>7.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -677,12 +677,12 @@
         <v>7.1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -697,7 +697,7 @@
         <v>6.8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Figure working with correct line breaks
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1152F784-4D48-46DB-B73E-F46578F1570F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94595FD1-6DF4-4BBE-841B-F036633462C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
@@ -111,15 +111,9 @@
     <t>C. Low Lake Powell releases + gains  through Grand Canyon</t>
   </si>
   <si>
-    <t>D. 85%, 65%, and 50% of 2000 to 2018  average flow</t>
-  </si>
-  <si>
     <t>E. Reclamation's Post 2026  web tool</t>
   </si>
   <si>
-    <t>F. Lowest consecutive flows in Reclamation's  ensembles and traces</t>
-  </si>
-  <si>
     <t>Cap depletions to 10-year lookback  period of flow.</t>
   </si>
   <si>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>Release to prevent drawdown  to 3,490 feet.</t>
+  </si>
+  <si>
+    <t>F. Lowest consecutive flows in  Reclamation's ensembles and traces</t>
+  </si>
+  <si>
+    <t>D. 85%, 65%, and 50% of  2000 to 2018 average flow</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -559,7 +559,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -579,12 +579,12 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
@@ -599,12 +599,12 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -619,12 +619,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Combine Flow Location and Flow Type into single column
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94595FD1-6DF4-4BBE-841B-F036633462C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47057F-8204-47BB-AB21-52DDD3A3687F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Flow Type</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Minimum (maf)</t>
   </si>
   <si>
-    <t>Regulated</t>
-  </si>
-  <si>
     <t>Natural</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Flow Location</t>
   </si>
   <si>
-    <t>Glen Canyon Dam</t>
-  </si>
-  <si>
     <t>Release</t>
   </si>
   <si>
@@ -133,6 +127,9 @@
   </si>
   <si>
     <t>D. 85%, 65%, and 50% of  2000 to 2018 average flow</t>
+  </si>
+  <si>
+    <t>Regulated Inflow</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,10 +501,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -516,21 +513,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
         <v>5</v>
@@ -539,18 +536,18 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -559,18 +556,18 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D4" s="5">
         <v>7</v>
@@ -579,18 +576,18 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5">
         <v>6</v>
@@ -599,18 +596,18 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="5">
         <v>4</v>
@@ -619,18 +616,18 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -642,13 +639,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <v>5</v>
@@ -657,18 +654,18 @@
         <v>7.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5">
         <v>4.0999999999999996</v>
@@ -677,18 +674,18 @@
         <v>7.1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5">
         <v>3.9</v>
@@ -697,7 +694,7 @@
         <v>6.8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -717,18 +714,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finished plot with legend on top
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47057F-8204-47BB-AB21-52DDD3A3687F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF88D3A-F496-4341-8361-4503A817CDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,12 +102,6 @@
     <t>B. Collaborator choices in immersive  modeling sessions</t>
   </si>
   <si>
-    <t>C. Low Lake Powell releases + gains  through Grand Canyon</t>
-  </si>
-  <si>
-    <t>E. Reclamation's Post 2026  web tool</t>
-  </si>
-  <si>
     <t>Cap depletions to 10-year lookback  period of flow.</t>
   </si>
   <si>
@@ -123,13 +117,19 @@
     <t>Release to prevent drawdown  to 3,490 feet.</t>
   </si>
   <si>
-    <t>F. Lowest consecutive flows in  Reclamation's ensembles and traces</t>
-  </si>
-  <si>
-    <t>D. 85%, 65%, and 50% of  2000 to 2018 average flow</t>
-  </si>
-  <si>
     <t>Regulated Inflow</t>
+  </si>
+  <si>
+    <t>C. 85%, 65%, and 50% of  2000 to 2018 average flow</t>
+  </si>
+  <si>
+    <t>D. Reclamation's Post 2026  web tool</t>
+  </si>
+  <si>
+    <t>E. Low Lake Powell releases + gains  through Grand Canyon</t>
+  </si>
+  <si>
+    <t>$Flo</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +536,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -556,72 +556,72 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="5">
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
         <v>6</v>
       </c>
-      <c r="E5" s="5">
-        <v>10</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Add 2 new lines for methods and strategies
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF88D3A-F496-4341-8361-4503A817CDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8BD1FC-6B9F-4484-B7F0-DF369E9519BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Extreme Low Flow Method</t>
   </si>
   <si>
-    <t>A. From tree rings back to 1400 AD</t>
-  </si>
-  <si>
     <t>Strategy to Stabilize Lake Levels</t>
   </si>
   <si>
@@ -99,37 +96,40 @@
     <t>F3. 3-year</t>
   </si>
   <si>
-    <t>B. Collaborator choices in immersive  modeling sessions</t>
-  </si>
-  <si>
-    <t>Cap depletions to 10-year lookback  period of flow.</t>
-  </si>
-  <si>
-    <t>Divide inflow; Users consume and conserve  within their account balance.</t>
-  </si>
-  <si>
-    <t>Rule curve; Consumption equals or less  than inflow minus evaporation.</t>
-  </si>
-  <si>
-    <t>Release 95% of regulated  inflow.</t>
-  </si>
-  <si>
-    <t>Release to prevent drawdown  to 3,490 feet.</t>
-  </si>
-  <si>
     <t>Regulated Inflow</t>
   </si>
   <si>
-    <t>C. 85%, 65%, and 50% of  2000 to 2018 average flow</t>
-  </si>
-  <si>
-    <t>D. Reclamation's Post 2026  web tool</t>
-  </si>
-  <si>
-    <t>E. Low Lake Powell releases + gains  through Grand Canyon</t>
-  </si>
-  <si>
-    <t>$Flo</t>
+    <t>A. From tree rings back to:1400 AD</t>
+  </si>
+  <si>
+    <t>Cap depletions to 10-year lookback:period of flow.</t>
+  </si>
+  <si>
+    <t>B. Collaborator choices in:immersive modeling:sessions</t>
+  </si>
+  <si>
+    <t>Divide inflow; Users consume and:conserve within their:account balance.</t>
+  </si>
+  <si>
+    <t>C. 85%, 65%, and 50% of:2000 to 2018:average flow</t>
+  </si>
+  <si>
+    <t>Release 95% of regulated:inflow.</t>
+  </si>
+  <si>
+    <t>D. Reclamation's:Post 2026:web tool</t>
+  </si>
+  <si>
+    <t>Release to prevent drawdown:to 3,490 feet.</t>
+  </si>
+  <si>
+    <t>E. Low Lake Powell releases:+ gains through:Grand Canyon</t>
+  </si>
+  <si>
+    <t>F. Lowest consecutive flows:in Reclamation's ensembles:and traces</t>
+  </si>
+  <si>
+    <t>Rule curve; Consumption equals or:less than inflow minus:evaporation.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,15 +513,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -556,18 +556,18 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D4" s="5">
         <v>6</v>
@@ -576,15 +576,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
@@ -596,18 +596,18 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5">
         <v>7</v>
@@ -616,12 +616,12 @@
         <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -654,12 +654,12 @@
         <v>7.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -674,12 +674,12 @@
         <v>7.1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -694,7 +694,7 @@
         <v>6.8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update left labels on all extreme flow diagrams
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8BD1FC-6B9F-4484-B7F0-DF369E9519BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69B8FCD-70C0-468E-832E-188555BAC7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
@@ -99,37 +99,37 @@
     <t>Regulated Inflow</t>
   </si>
   <si>
-    <t>A. From tree rings back to:1400 AD</t>
-  </si>
-  <si>
     <t>Cap depletions to 10-year lookback:period of flow.</t>
   </si>
   <si>
-    <t>B. Collaborator choices in:immersive modeling:sessions</t>
-  </si>
-  <si>
     <t>Divide inflow; Users consume and:conserve within their:account balance.</t>
   </si>
   <si>
-    <t>C. 85%, 65%, and 50% of:2000 to 2018:average flow</t>
-  </si>
-  <si>
     <t>Release 95% of regulated:inflow.</t>
   </si>
   <si>
-    <t>D. Reclamation's:Post 2026:web tool</t>
-  </si>
-  <si>
     <t>Release to prevent drawdown:to 3,490 feet.</t>
   </si>
   <si>
-    <t>E. Low Lake Powell releases:+ gains through:Grand Canyon</t>
-  </si>
-  <si>
-    <t>F. Lowest consecutive flows:in Reclamation's ensembles:and traces</t>
-  </si>
-  <si>
     <t>Rule curve; Consumption equals or:less than inflow minus:evaporation.</t>
+  </si>
+  <si>
+    <t>A. From tree rings back to:1400 AD (2023)</t>
+  </si>
+  <si>
+    <t>B. Collaborator choices in:immersive modeling:sessions (2021)</t>
+  </si>
+  <si>
+    <t>C. 85%, 65%, and 50% of:2000 to 2018:average flow (2022)</t>
+  </si>
+  <si>
+    <t>E. Low Lake Powell releases:+ gains through:Grand Canyon (2025)</t>
+  </si>
+  <si>
+    <t>F. Lowest consecutive flows:in Reclamation's ensembles:and traces (2025)</t>
+  </si>
+  <si>
+    <t>D. Release to prevent:drawdown to 3,490 feet:(2024).</t>
   </si>
 </sst>
 </file>
@@ -486,12 +486,12 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" customWidth="1"/>
+    <col min="1" max="1" width="49.08984375" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" customWidth="1"/>
     <col min="3" max="3" width="11.6328125" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" customWidth="1"/>
@@ -521,7 +521,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -536,12 +536,12 @@
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -556,12 +556,12 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -576,12 +576,12 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -596,7 +596,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -616,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated filter with line breaks on methods
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69B8FCD-70C0-468E-832E-188555BAC7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48F018D-7974-4DD8-87BF-5A7EB963D4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
@@ -120,16 +120,16 @@
     <t>B. Collaborator choices in:immersive modeling:sessions (2021)</t>
   </si>
   <si>
-    <t>C. 85%, 65%, and 50% of:2000 to 2018:average flow (2022)</t>
-  </si>
-  <si>
-    <t>E. Low Lake Powell releases:+ gains through:Grand Canyon (2025)</t>
-  </si>
-  <si>
     <t>F. Lowest consecutive flows:in Reclamation's ensembles:and traces (2025)</t>
   </si>
   <si>
     <t>D. Release to prevent:drawdown to 3,490 feet:(2024).</t>
+  </si>
+  <si>
+    <t>C. 85%, 65%, and 50% of:2000 to 2018 average:flow (2022)</t>
+  </si>
+  <si>
+    <t>E. Low Lake Powell:releases + gains through:Grand Canyon (2025)</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -561,7 +561,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Move Anabelles work to first method
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48F018D-7974-4DD8-87BF-5A7EB963D4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670E392A-7D27-40CF-A106-6C68E54E92AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Flow Type</t>
   </si>
@@ -87,15 +87,6 @@
     <t>Maximum (maf)</t>
   </si>
   <si>
-    <t>F1. 10-year</t>
-  </si>
-  <si>
-    <t>F2. 4-year</t>
-  </si>
-  <si>
-    <t>F3. 3-year</t>
-  </si>
-  <si>
     <t>Regulated Inflow</t>
   </si>
   <si>
@@ -114,22 +105,28 @@
     <t>Rule curve; Consumption equals or:less than inflow minus:evaporation.</t>
   </si>
   <si>
-    <t>A. From tree rings back to:1400 AD (2023)</t>
-  </si>
-  <si>
-    <t>B. Collaborator choices in:immersive modeling:sessions (2021)</t>
-  </si>
-  <si>
-    <t>F. Lowest consecutive flows:in Reclamation's ensembles:and traces (2025)</t>
-  </si>
-  <si>
-    <t>D. Release to prevent:drawdown to 3,490 feet:(2024).</t>
-  </si>
-  <si>
-    <t>C. 85%, 65%, and 50% of:2000 to 2018 average:flow (2022)</t>
-  </si>
-  <si>
-    <t>E. Low Lake Powell:releases + gains through:Grand Canyon (2025)</t>
+    <t>A. Lowest consecutive flows:in Reclamation's ensembles:and traces (2025)</t>
+  </si>
+  <si>
+    <t>A1. 10-year</t>
+  </si>
+  <si>
+    <t>A2. 3-year</t>
+  </si>
+  <si>
+    <t>B. From tree rings back to:1400 AD (2023)</t>
+  </si>
+  <si>
+    <t>C. Collaborator choices in:immersive modeling:sessions (2021)</t>
+  </si>
+  <si>
+    <t>D. 85%, 65%, and 50% of:2000 to 2018 average:flow (2022)</t>
+  </si>
+  <si>
+    <t>E. Release to prevent:drawdown to 3,490 feet:(2024).</t>
+  </si>
+  <si>
+    <t>F. Low Lake Powell:releases + gains through:Grand Canyon (2022)</t>
   </si>
 </sst>
 </file>
@@ -179,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -202,6 +199,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,9 +519,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -530,18 +530,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -550,73 +548,73 @@
         <v>2</v>
       </c>
       <c r="D3" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="5">
-        <v>13</v>
+        <v>7.5</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5">
-        <v>6</v>
+        <v>3.9</v>
       </c>
       <c r="E4" s="5">
-        <v>10</v>
+        <v>6.8</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5">
-        <v>6</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5">
-        <v>7</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -624,77 +622,59 @@
         <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="5">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5">
-        <v>4.0999999999999996</v>
-      </c>
       <c r="E9" s="5">
-        <v>7.1</v>
+        <v>10</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="5">
-        <v>3.9</v>
-      </c>
-      <c r="E10" s="5">
-        <v>6.8</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add legend to figure and adjust left axis labels
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670E392A-7D27-40CF-A106-6C68E54E92AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746FEE6C-8E14-4927-A75A-3660EA7DF075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Flow Type</t>
   </si>
@@ -105,15 +105,6 @@
     <t>Rule curve; Consumption equals or:less than inflow minus:evaporation.</t>
   </si>
   <si>
-    <t>A. Lowest consecutive flows:in Reclamation's ensembles:and traces (2025)</t>
-  </si>
-  <si>
-    <t>A1. 10-year</t>
-  </si>
-  <si>
-    <t>A2. 3-year</t>
-  </si>
-  <si>
     <t>B. From tree rings back to:1400 AD (2023)</t>
   </si>
   <si>
@@ -127,6 +118,12 @@
   </si>
   <si>
     <t>F. Low Lake Powell:releases + gains through:Grand Canyon (2022)</t>
+  </si>
+  <si>
+    <t>A2. Lowest 3-year average:flows</t>
+  </si>
+  <si>
+    <t>A1. Lowest 10-year average flows:in Reclamation's post-:2026 ensembles and:traces (2025)</t>
   </si>
 </sst>
 </file>
@@ -176,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -196,12 +193,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,9 +510,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -530,16 +521,18 @@
         <v>2</v>
       </c>
       <c r="D2" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+        <v>7.5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -548,18 +541,18 @@
         <v>2</v>
       </c>
       <c r="D3" s="5">
-        <v>5</v>
+        <v>3.9</v>
       </c>
       <c r="E3" s="5">
-        <v>7.5</v>
+        <v>6.8</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -568,18 +561,18 @@
         <v>2</v>
       </c>
       <c r="D4" s="5">
-        <v>3.9</v>
+        <v>5</v>
       </c>
       <c r="E4" s="5">
-        <v>6.8</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -588,92 +581,72 @@
         <v>2</v>
       </c>
       <c r="D5" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="5">
-        <v>10</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5">
-        <v>10</v>
-      </c>
-      <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ExtremeLowFlow blog post MSWORD and PDF
</commit_message>
<xml_diff>
--- a/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
+++ b/ColoradoRiverExtremeLowFlowScenariosAll/ColoradoRiverExtremeLowFlowScenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ColoradoRiverExtremeLowFlowScenariosAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746FEE6C-8E14-4927-A75A-3660EA7DF075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D655FE-AAD8-4F3D-B442-98E0DFCDEB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtremeFlows" sheetId="1" r:id="rId1"/>
@@ -105,25 +105,25 @@
     <t>Rule curve; Consumption equals or:less than inflow minus:evaporation.</t>
   </si>
   <si>
-    <t>B. From tree rings back to:1400 AD (2023)</t>
-  </si>
-  <si>
-    <t>C. Collaborator choices in:immersive modeling:sessions (2021)</t>
-  </si>
-  <si>
-    <t>D. 85%, 65%, and 50% of:2000 to 2018 average:flow (2022)</t>
-  </si>
-  <si>
     <t>E. Release to prevent:drawdown to 3,490 feet:(2024).</t>
   </si>
   <si>
-    <t>F. Low Lake Powell:releases + gains through:Grand Canyon (2022)</t>
-  </si>
-  <si>
-    <t>A2. Lowest 3-year average:flows</t>
-  </si>
-  <si>
-    <t>A1. Lowest 10-year average flows:in Reclamation's post-:2026 ensembles and:traces (2025)</t>
+    <t>A1. Lowest 10-year average flows:in Reclamation's post-:2026 ensembles and:traces (2025).</t>
+  </si>
+  <si>
+    <t>B. From tree rings back to:1400 AD (2023).</t>
+  </si>
+  <si>
+    <t>C. Collaborator choices in:immersive modeling:sessions (2021).</t>
+  </si>
+  <si>
+    <t>D. 85%, 65%, and 50% of:2000 to 2018 average:flow (2022).</t>
+  </si>
+  <si>
+    <t>F. Low Lake Powell:releases + gains through:Grand Canyon (2022).</t>
+  </si>
+  <si>
+    <t>A2. Low annual flows within the:10-year periods (2025).</t>
   </si>
 </sst>
 </file>
@@ -476,9 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -512,7 +510,7 @@
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -532,7 +530,7 @@
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -541,10 +539,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="5">
-        <v>3.9</v>
+        <v>3</v>
       </c>
       <c r="E3" s="5">
-        <v>6.8</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
@@ -552,7 +550,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -572,7 +570,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -592,7 +590,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>14</v>
@@ -612,7 +610,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
@@ -632,7 +630,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>

</xml_diff>